<commit_message>
range_door_light fix - command on istead red/green
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="284">
   <si>
     <t>Описание логических устройств, принимаемых ими команд, и выдаваемых ими репортов, а также состояний</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>range_door_light</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
   <si>
     <t>Крыса</t>
@@ -1289,8 +1292,8 @@
   </sheetPr>
   <dimension ref="A1:U113"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K45" activeCellId="0" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2567,7 +2570,7 @@
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="12" t="s">
         <v>31</v>
@@ -3142,10 +3145,12 @@
         <v>1</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
+      <c r="N44" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
@@ -3171,12 +3176,8 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
-      <c r="K45" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>98</v>
-      </c>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
       <c r="O45" s="12"/>
@@ -3198,10 +3199,10 @@
         <v>20</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>28</v>
@@ -3230,20 +3231,20 @@
         <v>0</v>
       </c>
       <c r="P46" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q46" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T46" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="U46" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3269,10 +3270,10 @@
         <v>1</v>
       </c>
       <c r="T47" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="U47" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3280,10 +3281,10 @@
         <v>21</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>28</v>
@@ -3364,10 +3365,10 @@
         <v>22</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>28</v>
@@ -3396,20 +3397,20 @@
         <v>0</v>
       </c>
       <c r="P50" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q50" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R50" s="12"/>
       <c r="S50" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T50" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U50" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,10 +3436,10 @@
         <v>1</v>
       </c>
       <c r="T51" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U51" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3446,10 +3447,10 @@
         <v>23</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>28</v>
@@ -3528,10 +3529,10 @@
         <v>23</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>28</v>
@@ -3612,10 +3613,10 @@
         <v>23</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>28</v>
@@ -3696,10 +3697,10 @@
         <v>22</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>28</v>
@@ -3735,7 +3736,7 @@
         <v>72</v>
       </c>
       <c r="Q58" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R58" s="12"/>
       <c r="S58" s="13" t="n">
@@ -3782,10 +3783,10 @@
         <v>24</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>28</v>
@@ -3825,7 +3826,7 @@
         <v>29</v>
       </c>
       <c r="U60" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3858,7 +3859,7 @@
         <v>31</v>
       </c>
       <c r="U61" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3866,10 +3867,10 @@
         <v>25</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>28</v>
@@ -3950,10 +3951,10 @@
         <v>26</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>28</v>
@@ -4034,10 +4035,10 @@
         <v>27</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>28</v>
@@ -4118,10 +4119,10 @@
         <v>28</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>28</v>
@@ -4150,20 +4151,20 @@
         <v>0</v>
       </c>
       <c r="P68" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q68" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R68" s="12"/>
       <c r="S68" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T68" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U68" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4189,10 +4190,10 @@
         <v>1</v>
       </c>
       <c r="T69" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U69" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4200,10 +4201,10 @@
         <v>29</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>28</v>
@@ -4232,20 +4233,20 @@
         <v>0</v>
       </c>
       <c r="P70" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q70" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R70" s="12"/>
       <c r="S70" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T70" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="U70" s="13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4271,10 +4272,10 @@
         <v>1</v>
       </c>
       <c r="T71" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="U71" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4282,10 +4283,10 @@
         <v>30</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>28</v>
@@ -4310,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="L72" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M72" s="12"/>
       <c r="N72" s="12"/>
@@ -4321,17 +4322,17 @@
         <v>72</v>
       </c>
       <c r="Q72" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R72" s="12"/>
       <c r="S72" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T72" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="U72" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4349,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="L73" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M73" s="12"/>
       <c r="N73" s="12"/>
@@ -4361,10 +4362,10 @@
         <v>1</v>
       </c>
       <c r="T73" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U73" s="13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,10 +4373,10 @@
         <v>31</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>28</v>
@@ -4400,7 +4401,7 @@
         <v>0</v>
       </c>
       <c r="L74" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M74" s="12"/>
       <c r="N74" s="12"/>
@@ -4411,17 +4412,17 @@
         <v>72</v>
       </c>
       <c r="Q74" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R74" s="12"/>
       <c r="S74" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T74" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="U74" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4439,7 +4440,7 @@
         <v>1</v>
       </c>
       <c r="L75" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M75" s="12"/>
       <c r="N75" s="12"/>
@@ -4451,10 +4452,10 @@
         <v>1</v>
       </c>
       <c r="T75" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U75" s="13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,10 +4463,10 @@
         <v>32</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>28</v>
@@ -4490,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M76" s="12"/>
       <c r="N76" s="12"/>
@@ -4501,17 +4502,17 @@
         <v>72</v>
       </c>
       <c r="Q76" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R76" s="12"/>
       <c r="S76" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T76" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="U76" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4529,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="L77" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M77" s="12"/>
       <c r="N77" s="12"/>
@@ -4541,10 +4542,10 @@
         <v>1</v>
       </c>
       <c r="T77" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U77" s="13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4552,10 +4553,10 @@
         <v>33</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>28</v>
@@ -4636,10 +4637,10 @@
         <v>34</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>28</v>
@@ -4679,7 +4680,7 @@
         <v>29</v>
       </c>
       <c r="U80" s="13" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4712,7 +4713,7 @@
         <v>31</v>
       </c>
       <c r="U81" s="13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4720,10 +4721,10 @@
         <v>35</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>28</v>
@@ -4804,10 +4805,10 @@
         <v>36</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D84" s="12" t="s">
         <v>28</v>
@@ -4832,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="L84" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M84" s="12"/>
       <c r="N84" s="12"/>
@@ -4840,20 +4841,20 @@
         <v>0</v>
       </c>
       <c r="P84" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q84" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R84" s="12"/>
       <c r="S84" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T84" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U84" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4871,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="L85" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M85" s="12"/>
       <c r="N85" s="12"/>
@@ -4883,10 +4884,10 @@
         <v>1</v>
       </c>
       <c r="T85" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U85" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4894,10 +4895,10 @@
         <v>37</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D86" s="12" t="s">
         <v>28</v>
@@ -4922,17 +4923,17 @@
         <v>1</v>
       </c>
       <c r="L86" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M86" s="12"/>
       <c r="N86" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O86" s="12" t="n">
         <v>0</v>
       </c>
       <c r="P86" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Q86" s="12" t="s">
         <v>86</v>
@@ -4942,10 +4943,10 @@
         <v>1</v>
       </c>
       <c r="T86" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="U86" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4963,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M87" s="12"/>
       <c r="N87" s="12"/>
@@ -4975,10 +4976,10 @@
         <v>0</v>
       </c>
       <c r="T87" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="U87" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4986,10 +4987,10 @@
         <v>38</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>28</v>
@@ -5014,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="L88" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M88" s="12"/>
       <c r="N88" s="12"/>
@@ -5022,20 +5023,20 @@
         <v>0</v>
       </c>
       <c r="P88" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q88" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R88" s="12"/>
       <c r="S88" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T88" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="U88" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5053,11 +5054,11 @@
         <v>1</v>
       </c>
       <c r="L89" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M89" s="12"/>
       <c r="N89" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O89" s="12"/>
       <c r="P89" s="12"/>
@@ -5067,10 +5068,10 @@
         <v>1</v>
       </c>
       <c r="T89" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U89" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5088,7 +5089,7 @@
         <v>3</v>
       </c>
       <c r="L90" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M90" s="12"/>
       <c r="N90" s="12"/>
@@ -5096,20 +5097,20 @@
         <v>3</v>
       </c>
       <c r="P90" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Q90" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="R90" s="12"/>
       <c r="S90" s="13" t="n">
         <v>2</v>
       </c>
       <c r="T90" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U90" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,11 +5128,11 @@
         <v>2</v>
       </c>
       <c r="L91" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M91" s="12"/>
       <c r="N91" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O91" s="12"/>
       <c r="P91" s="12"/>
@@ -5141,10 +5142,10 @@
         <v>3</v>
       </c>
       <c r="T91" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U91" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5152,10 +5153,10 @@
         <v>39</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D92" s="12" t="s">
         <v>28</v>
@@ -5180,7 +5181,7 @@
         <v>0</v>
       </c>
       <c r="L92" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M92" s="12"/>
       <c r="N92" s="12"/>
@@ -5188,20 +5189,20 @@
         <v>0</v>
       </c>
       <c r="P92" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q92" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R92" s="12"/>
       <c r="S92" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T92" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="U92" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5219,11 +5220,11 @@
         <v>1</v>
       </c>
       <c r="L93" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M93" s="12"/>
       <c r="N93" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O93" s="12"/>
       <c r="P93" s="12"/>
@@ -5233,10 +5234,10 @@
         <v>1</v>
       </c>
       <c r="T93" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U93" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5254,7 +5255,7 @@
         <v>3</v>
       </c>
       <c r="L94" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M94" s="12"/>
       <c r="N94" s="12"/>
@@ -5262,20 +5263,20 @@
         <v>3</v>
       </c>
       <c r="P94" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Q94" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="R94" s="12"/>
       <c r="S94" s="13" t="n">
         <v>2</v>
       </c>
       <c r="T94" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U94" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,11 +5294,11 @@
         <v>2</v>
       </c>
       <c r="L95" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M95" s="12"/>
       <c r="N95" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O95" s="12"/>
       <c r="P95" s="12"/>
@@ -5307,10 +5308,10 @@
         <v>3</v>
       </c>
       <c r="T95" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U95" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5318,10 +5319,10 @@
         <v>40</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>28</v>
@@ -5346,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="L96" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M96" s="12"/>
       <c r="N96" s="12"/>
@@ -5354,20 +5355,20 @@
         <v>0</v>
       </c>
       <c r="P96" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q96" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R96" s="12"/>
       <c r="S96" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T96" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="U96" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5385,11 +5386,11 @@
         <v>1</v>
       </c>
       <c r="L97" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M97" s="12"/>
       <c r="N97" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O97" s="12"/>
       <c r="P97" s="12"/>
@@ -5399,10 +5400,10 @@
         <v>1</v>
       </c>
       <c r="T97" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U97" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5420,7 +5421,7 @@
         <v>3</v>
       </c>
       <c r="L98" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M98" s="12"/>
       <c r="N98" s="12"/>
@@ -5428,20 +5429,20 @@
         <v>3</v>
       </c>
       <c r="P98" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Q98" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="R98" s="12"/>
       <c r="S98" s="13" t="n">
         <v>2</v>
       </c>
       <c r="T98" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U98" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5459,11 +5460,11 @@
         <v>2</v>
       </c>
       <c r="L99" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M99" s="12"/>
       <c r="N99" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O99" s="12"/>
       <c r="P99" s="12"/>
@@ -5473,10 +5474,10 @@
         <v>3</v>
       </c>
       <c r="T99" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U99" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5484,10 +5485,10 @@
         <v>41</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D100" s="12" t="s">
         <v>28</v>
@@ -5512,7 +5513,7 @@
         <v>0</v>
       </c>
       <c r="L100" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M100" s="12"/>
       <c r="N100" s="12"/>
@@ -5520,20 +5521,20 @@
         <v>0</v>
       </c>
       <c r="P100" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q100" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R100" s="12"/>
       <c r="S100" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T100" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="U100" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5551,11 +5552,11 @@
         <v>1</v>
       </c>
       <c r="L101" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M101" s="12"/>
       <c r="N101" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O101" s="12"/>
       <c r="P101" s="12"/>
@@ -5565,10 +5566,10 @@
         <v>1</v>
       </c>
       <c r="T101" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U101" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5586,7 +5587,7 @@
         <v>3</v>
       </c>
       <c r="L102" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M102" s="12"/>
       <c r="N102" s="12"/>
@@ -5594,20 +5595,20 @@
         <v>3</v>
       </c>
       <c r="P102" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Q102" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="R102" s="12"/>
       <c r="S102" s="13" t="n">
         <v>2</v>
       </c>
       <c r="T102" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U102" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5625,11 +5626,11 @@
         <v>2</v>
       </c>
       <c r="L103" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M103" s="12"/>
       <c r="N103" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O103" s="12"/>
       <c r="P103" s="12"/>
@@ -5639,10 +5640,10 @@
         <v>3</v>
       </c>
       <c r="T103" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U103" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5650,10 +5651,10 @@
         <v>42</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D104" s="12" t="s">
         <v>28</v>
@@ -5678,7 +5679,7 @@
         <v>0</v>
       </c>
       <c r="L104" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M104" s="12"/>
       <c r="N104" s="12"/>
@@ -5686,20 +5687,20 @@
         <v>0</v>
       </c>
       <c r="P104" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q104" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="R104" s="12"/>
       <c r="S104" s="13" t="n">
         <v>0</v>
       </c>
       <c r="T104" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U104" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5717,7 +5718,7 @@
         <v>1</v>
       </c>
       <c r="L105" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M105" s="12"/>
       <c r="N105" s="12"/>
@@ -5729,10 +5730,10 @@
         <v>1</v>
       </c>
       <c r="T105" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U105" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5740,10 +5741,10 @@
         <v>43</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D106" s="12" t="s">
         <v>28</v>
@@ -5768,11 +5769,11 @@
         <v>0</v>
       </c>
       <c r="L106" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M106" s="12"/>
       <c r="N106" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O106" s="12"/>
       <c r="P106" s="12"/>
@@ -5782,10 +5783,10 @@
         <v>0</v>
       </c>
       <c r="T106" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U106" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5803,11 +5804,11 @@
         <v>1</v>
       </c>
       <c r="L107" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M107" s="12"/>
       <c r="N107" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O107" s="12"/>
       <c r="P107" s="12"/>
@@ -5817,10 +5818,10 @@
         <v>1</v>
       </c>
       <c r="T107" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U107" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5828,10 +5829,10 @@
         <v>44</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D108" s="12" t="s">
         <v>28</v>
@@ -5856,11 +5857,11 @@
         <v>0</v>
       </c>
       <c r="L108" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M108" s="12"/>
       <c r="N108" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O108" s="12"/>
       <c r="P108" s="12"/>
@@ -5870,10 +5871,10 @@
         <v>0</v>
       </c>
       <c r="T108" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U108" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5891,11 +5892,11 @@
         <v>1</v>
       </c>
       <c r="L109" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M109" s="12"/>
       <c r="N109" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O109" s="12"/>
       <c r="P109" s="12"/>
@@ -5905,10 +5906,10 @@
         <v>1</v>
       </c>
       <c r="T109" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U109" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5916,10 +5917,10 @@
         <v>45</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D110" s="12" t="s">
         <v>28</v>
@@ -5944,11 +5945,11 @@
         <v>0</v>
       </c>
       <c r="L110" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M110" s="12"/>
       <c r="N110" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O110" s="12"/>
       <c r="P110" s="12"/>
@@ -5958,10 +5959,10 @@
         <v>0</v>
       </c>
       <c r="T110" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U110" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5979,11 +5980,11 @@
         <v>1</v>
       </c>
       <c r="L111" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M111" s="12"/>
       <c r="N111" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O111" s="12"/>
       <c r="P111" s="12"/>
@@ -5993,10 +5994,10 @@
         <v>1</v>
       </c>
       <c r="T111" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U111" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6004,10 +6005,10 @@
         <v>46</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D112" s="12" t="s">
         <v>28</v>
@@ -6032,11 +6033,11 @@
         <v>0</v>
       </c>
       <c r="L112" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M112" s="12"/>
       <c r="N112" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O112" s="12"/>
       <c r="P112" s="12"/>
@@ -6046,10 +6047,10 @@
         <v>0</v>
       </c>
       <c r="T112" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U112" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6067,11 +6068,11 @@
         <v>1</v>
       </c>
       <c r="L113" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M113" s="12"/>
       <c r="N113" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O113" s="12"/>
       <c r="P113" s="12"/>
@@ -6081,10 +6082,10 @@
         <v>1</v>
       </c>
       <c r="T113" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U113" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -6860,7 +6861,7 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -6874,13 +6875,13 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="20" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
@@ -6895,7 +6896,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -6910,7 +6911,7 @@
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
@@ -6934,13 +6935,13 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="18" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="20" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -6955,7 +6956,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -6970,7 +6971,7 @@
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
       <c r="F7" s="26" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
@@ -6980,13 +6981,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6994,7 +6995,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7002,7 +7003,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -7023,7 +7024,7 @@
   </sheetPr>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -7071,7 +7072,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7079,7 +7080,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7087,7 +7088,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7095,7 +7096,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7103,7 +7104,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7111,7 +7112,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7119,7 +7120,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7127,7 +7128,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7135,7 +7136,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7155,7 +7156,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7166,7 +7167,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7174,7 +7175,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7182,7 +7183,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7190,7 +7191,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7198,7 +7199,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7206,7 +7207,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,7 +7215,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7222,7 +7223,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7230,7 +7231,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,7 +7239,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7246,7 +7247,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7254,7 +7255,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7262,10 +7263,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7273,7 +7274,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7281,7 +7282,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7289,21 +7290,21 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10"/>
       <c r="B68" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7311,7 +7312,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7319,7 +7320,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7327,7 +7328,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7341,7 +7342,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7355,7 +7356,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7369,7 +7370,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7383,7 +7384,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7391,7 +7392,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>